<commit_message>
Refine the code for data collection
</commit_message>
<xml_diff>
--- a/Results/Perbandingan Transformers dan Neural Network.xlsx
+++ b/Results/Perbandingan Transformers dan Neural Network.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="45">
   <si>
     <t xml:space="preserve">Device Used</t>
   </si>
@@ -69,6 +69,9 @@
     <t xml:space="preserve">Processing Time (ms)</t>
   </si>
   <si>
+    <t xml:space="preserve">Average Processing Time (ms)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Neural Network</t>
   </si>
   <si>
@@ -133,14 +136,36 @@
   </si>
   <si>
     <t xml:space="preserve">Okay I see. Enjoy the rest of your day then</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi there. What brings you here today?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello there. Glad to see you're back. What's going on in your world right now?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello there. Tell me how are you feeling today?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi there. How are you feeling today?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'm here for you. Could you tell me why you're feeling this way?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great to see you. How do you feel currently?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Okay we're done. Have a great day</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -221,7 +246,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -243,6 +268,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -269,9 +298,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>375120</xdr:colOff>
+      <xdr:colOff>374760</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -280,13 +309,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:srcRect l="0" t="0" r="32031" b="0"/>
+        <a:srcRect l="0" t="0" r="32025" b="0"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="78840" y="1843560"/>
-          <a:ext cx="4816800" cy="8244000"/>
+          <a:ext cx="4821480" cy="8243640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -307,9 +336,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>481320</xdr:colOff>
+      <xdr:colOff>480960</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -318,13 +347,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId2"/>
-        <a:srcRect l="71483" t="0" r="0" b="0"/>
+        <a:srcRect l="71477" t="0" r="0" b="0"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7052040" y="1777320"/>
-          <a:ext cx="2020320" cy="8244000"/>
+          <a:off x="7061040" y="1777320"/>
+          <a:ext cx="2022120" cy="8243640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -346,11 +375,11 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.92"/>
   </cols>
@@ -422,20 +451,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="27.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="23.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="29.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="23.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="4" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="29.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="29.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="29.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="4" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -452,225 +483,360 @@
         <v>15</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>14</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>9</v>
       </c>
+      <c r="D2" s="6" t="n">
+        <f aca="false">AVERAGE(C2:C6)</f>
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6" t="n">
+        <f aca="false">AVERAGE(F2:F6)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="D3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>28</v>
       </c>
+      <c r="D4" s="6"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="D5" s="6"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>33</v>
       </c>
+      <c r="D6" s="6"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>24</v>
       </c>
+      <c r="D7" s="6" t="n">
+        <f aca="false">AVERAGE(C7:C11)</f>
+        <v>22.8</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <f aca="false">AVERAGE(F7:F11)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>24</v>
       </c>
+      <c r="D8" s="6"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>20</v>
       </c>
+      <c r="D9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>24</v>
       </c>
+      <c r="D10" s="6"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>22</v>
       </c>
+      <c r="D11" s="6"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>27</v>
       </c>
+      <c r="D12" s="6" t="n">
+        <f aca="false">AVERAGE(C12:C16)</f>
+        <v>26.2</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <f aca="false">AVERAGE(F12:F16)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>26</v>
       </c>
+      <c r="D13" s="6"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>28</v>
       </c>
+      <c r="D14" s="6"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>25</v>
       </c>
+      <c r="D15" s="6"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>25</v>
       </c>
+      <c r="D16" s="6"/>
+      <c r="G16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>35</v>
       </c>
+      <c r="D17" s="6" t="n">
+        <f aca="false">AVERAGE(C17:C21)</f>
+        <v>24.2</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <f aca="false">AVERAGE(F17:F21)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>18</v>
       </c>
+      <c r="D18" s="6"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>13</v>
       </c>
+      <c r="D19" s="6"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>28</v>
       </c>
+      <c r="D20" s="6"/>
+      <c r="G20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C21" s="3" t="n">
         <v>27</v>
       </c>
+      <c r="D21" s="6"/>
+      <c r="G21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>24</v>
       </c>
+      <c r="D22" s="6" t="n">
+        <f aca="false">AVERAGE(C22:C26)</f>
+        <v>19.2</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="6" t="n">
+        <f aca="false">AVERAGE(F22:F26)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C23" s="3" t="n">
         <v>24</v>
       </c>
+      <c r="D23" s="6"/>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>16</v>
       </c>
+      <c r="D24" s="6"/>
+      <c r="G24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C25" s="3" t="n">
         <v>21</v>
       </c>
+      <c r="D25" s="6"/>
+      <c r="G25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>11</v>
       </c>
+      <c r="D26" s="6"/>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="3" t="n">
+        <f aca="false">AVERAGE(C2:C26)</f>
+        <v>22.08</v>
+      </c>
+      <c r="D27" s="3" t="n">
+        <f aca="false">AVERAGE(D2:D26)</f>
+        <v>22.08</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="3" t="n">
+        <f aca="false">AVERAGE(F2:F26)</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="3" t="n">
+        <f aca="false">AVERAGE(G2:G26)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="G2:G6"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="G12:G16"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="G17:G21"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="G22:G26"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -686,20 +852,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="27.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="27.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="23.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="29.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="23.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="4" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="29.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="29.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="29.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="4" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -716,79 +888,494 @@
         <v>15</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="6" t="n">
+        <f aca="false">AVERAGE(C2:C6)</f>
+        <v>23.6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="G2" s="6" t="n">
+        <f aca="false">AVERAGE(F2:F6)</f>
+        <v>40.8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="6"/>
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>25</v>
       </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="6"/>
+      <c r="E5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>23</v>
       </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="6" t="n">
+        <f aca="false">AVERAGE(C7:C11)</f>
+        <v>23.2</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <f aca="false">AVERAGE(F7:F11)</f>
+        <v>41.8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>43</v>
+      </c>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="n">
         <v>24</v>
       </c>
+      <c r="D12" s="6" t="n">
+        <f aca="false">AVERAGE(C12:C16)</f>
+        <v>23.2</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <f aca="false">AVERAGE(F12:F16)</f>
+        <v>41.6</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="G16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="D17" s="6" t="n">
+        <f aca="false">AVERAGE(C17:C21)</f>
+        <v>27.2</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <f aca="false">AVERAGE(F17:F21)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="D22" s="6" t="n">
+        <f aca="false">AVERAGE(C22:C26)</f>
+        <v>26.4</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="G22" s="6" t="n">
+        <f aca="false">AVERAGE(F22:F26)</f>
+        <v>42.2</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <v>43</v>
+      </c>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="3" t="n">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
-        <v>32</v>
+      <c r="D26" s="6"/>
+      <c r="E26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="3" t="n">
+        <v>43</v>
+      </c>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="3" t="n">
+        <f aca="false">AVERAGE(C2:C26)</f>
+        <v>24.72</v>
+      </c>
+      <c r="D27" s="3" t="n">
+        <f aca="false">AVERAGE(D2:D26)</f>
+        <v>24.72</v>
+      </c>
+      <c r="F27" s="3" t="n">
+        <f aca="false">AVERAGE(F2:F26)</f>
+        <v>41.48</v>
+      </c>
+      <c r="G27" s="3" t="n">
+        <f aca="false">AVERAGE(G2:G26)</f>
+        <v>41.48</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="G2:G6"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="G12:G16"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="G17:G21"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="G22:G26"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>